<commit_message>
word scaling analysis and file reading fixes
</commit_message>
<xml_diff>
--- a/New Analysis Code/Templates/Word Scaling Analysis Template.xlsx
+++ b/New Analysis Code/Templates/Word Scaling Analysis Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emban\Documents\GitHub\EMC-Scrotation-Station\New Analysis Code\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{922AD4D0-D946-485D-B2EE-20A6575E7D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6482DDB-1AC9-460D-8269-EC291D135601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Colors</t>
   </si>
@@ -64,9 +64,6 @@
     <t>Log2 of Height (log2 °)</t>
   </si>
   <si>
-    <t>0, 1, 2, 4, 8, 16, 32</t>
-  </si>
-  <si>
     <t>XTick Labels</t>
   </si>
   <si>
@@ -109,10 +106,7 @@
     <t>Absolute Value</t>
   </si>
   <si>
-    <t>Folder Names</t>
-  </si>
-  <si>
-    <t>Xtick spacing</t>
+    <t>Xtick Locations</t>
   </si>
 </sst>
 </file>
@@ -476,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -497,148 +491,136 @@
     <col min="12" max="12" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>15</v>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>0</v>
       </c>
       <c r="J1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
-        <v>16</v>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
       </c>
       <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2">
         <v>1</v>
       </c>
-      <c r="G2">
-        <v>4</v>
-      </c>
-      <c r="H2" s="2">
-        <v>1</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>14</v>
+      <c r="I2" t="s">
+        <v>18</v>
       </c>
       <c r="J2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:10">
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3">
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3">
         <v>3</v>
       </c>
-      <c r="G3">
-        <v>4</v>
+      <c r="I3" t="s">
+        <v>17</v>
       </c>
       <c r="J3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:10">
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4">
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4">
         <v>4</v>
       </c>
-      <c r="G4">
-        <v>4</v>
+      <c r="I4" t="s">
+        <v>24</v>
       </c>
       <c r="J4" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:10">
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5">
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5">
         <v>2</v>
       </c>
-      <c r="G5">
-        <v>4</v>
+      <c r="I5" t="s">
+        <v>19</v>
       </c>
       <c r="J5" t="s">
-        <v>20</v>
-      </c>
-      <c r="K5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:10">
       <c r="B6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:10">
       <c r="C15" s="1"/>
     </row>
   </sheetData>

</xml_diff>